<commit_message>
new commands fetch and pull
</commit_message>
<xml_diff>
--- a/Git learnings.xlsx
+++ b/Git learnings.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aloksingh/Documents/Github-Tutorial-Alok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623417AD-2536-4C43-A5E1-31298591F421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5E5269-C6DD-CA48-BDD9-7CF5510C2714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{A33BD040-1E14-2E45-91EB-0A91B5A7A573}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Home" sheetId="1" r:id="rId1"/>
     <sheet name="Installation" sheetId="3" r:id="rId2"/>
-    <sheet name="Hands-on 1st" sheetId="2" r:id="rId3"/>
-    <sheet name="Diff Excrcise 4" sheetId="7" r:id="rId4"/>
-    <sheet name="Merging Exercise 3" sheetId="6" r:id="rId5"/>
-    <sheet name="Branches Exercise 2" sheetId="5" r:id="rId6"/>
-    <sheet name="Basic Exercise 1" sheetId="4" r:id="rId7"/>
+    <sheet name="&lt;main&gt;Hands-on reference " sheetId="2" r:id="rId3"/>
+    <sheet name="Github Exercise 5" sheetId="8" r:id="rId4"/>
+    <sheet name="Diff Excrcise 4" sheetId="7" r:id="rId5"/>
+    <sheet name="Merging Exercise 3" sheetId="6" r:id="rId6"/>
+    <sheet name="Branches Exercise 2" sheetId="5" r:id="rId7"/>
+    <sheet name="Basic Exercise 1" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="244">
   <si>
     <t>https://www.canva.com/design/DAEQbZDcRTs/eoJbTLVE8BolmKIyFjGByQ/view?utm_content=DAEQbZDcRTs&amp;utm_campaign=designshare&amp;utm_medium=link&amp;utm_source=editor#8</t>
   </si>
@@ -1041,15 +1042,9 @@
     <t>v</t>
   </si>
   <si>
-    <t>fastforward merge, go to branch you want to merge to, and do merge</t>
-  </si>
-  <si>
     <t>git merge &lt;branch to be merged&gt;</t>
   </si>
   <si>
-    <t>ort merge, new branch developed but older branch is modified,GIT Will force to write a merge message</t>
-  </si>
-  <si>
     <t>Merging Branches</t>
   </si>
   <si>
@@ -1588,13 +1583,505 @@
   </si>
   <si>
     <t>git remote set-url origin git@github.com:OWNER/REPOSITORY.git</t>
+  </si>
+  <si>
+    <t>Github Basics Exercise</t>
+  </si>
+  <si>
+    <t>Create a new repository locally on your machine.</t>
+  </si>
+  <si>
+    <t>Create a new Github repository. Name it whatever you want.</t>
+  </si>
+  <si>
+    <t>Connect your local repo to the Github repo.</t>
+  </si>
+  <si>
+    <t>Optional: rename the default branch from master to main.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Make a new file called </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>favorites.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leave it empty. Make your first commit on the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Push up your </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch to Github! Make sure you see your empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>favorites.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file on Github.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Next, create two branches: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>foods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>movies</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Switch to the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>foods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch. Add three (or more) of your favorite foods to the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>favorites.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file. Add and commit your changes on the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>foods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Switch to the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>movies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch and add three or more of your favorite movies to the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>favorites.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file. Add and commit your changes on the movies branch.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Push up your </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>foods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch to Github. Make sure you see it on Github!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Push up your </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>movies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch to Github. Make sure you see it on Github!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Merge the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>foods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch into the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch. Then merge the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>movies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch into the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch. If necessary, resolve conflicts so that you end up with your favorite foods and favorite movies in the same </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>favorites.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Push up the latest work on your </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> branch to Github.</t>
+    </r>
+  </si>
+  <si>
+    <t>Fetch and Pull</t>
+  </si>
+  <si>
+    <t>Cloning and pushing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenarios when multiple people are working on project </t>
+  </si>
+  <si>
+    <t>we have 4 areas-&gt;</t>
+  </si>
+  <si>
+    <t>workspace</t>
+  </si>
+  <si>
+    <t>Staging</t>
+  </si>
+  <si>
+    <t>local repo</t>
+  </si>
+  <si>
+    <t>Remote Repo</t>
+  </si>
+  <si>
+    <t>-------------&gt;</t>
+  </si>
+  <si>
+    <t>---------&gt;</t>
+  </si>
+  <si>
+    <t>-----------&gt;</t>
+  </si>
+  <si>
+    <t>git add</t>
+  </si>
+  <si>
+    <t>git commit</t>
+  </si>
+  <si>
+    <t>git push</t>
+  </si>
+  <si>
+    <t>&lt;---------------git pull-------------------</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;--git fetch --------</t>
+  </si>
+  <si>
+    <t>Git fetch will bring changes from the branch to local repo but will not change your latest development work</t>
+  </si>
+  <si>
+    <t>git fetch origin master</t>
+  </si>
+  <si>
+    <t>Understanding difference between main and origin/main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">origin/ main is main branch in github, main is local main branch </t>
+  </si>
+  <si>
+    <t>Get help on any command</t>
+  </si>
+  <si>
+    <t>git -&lt;command e.g. branch&gt; --help</t>
+  </si>
+  <si>
+    <t>git pull will bring changes from remote repo and merge with the current branch we're on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git pull &lt;remote&gt; &lt;branch&gt; e.g. git </t>
+  </si>
+  <si>
+    <t>ort merge, new branch developed but older branch is modified,GIT Will force to write a merge message, might triggetr conflicts</t>
+  </si>
+  <si>
+    <t>Simplest case--&gt;fastforward merge, go to branch you want to merge to, and do merge. New branch has additional content which is not on main. Main catches up.</t>
+  </si>
+  <si>
+    <t>Git may not be able to do merges automatically e.g. when 2 branches have modified same file. This creates the connflict. Have to be manually resolved.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1666,6 +2153,12 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1675,7 +2168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1683,12 +2176,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -1702,6 +2210,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2153,7 +2679,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2188,16 +2714,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFA2FDF-9161-E540-A94F-75475D0D0289}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2257,7 +2784,12 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C8" s="4"/>
+      <c r="A8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -2295,10 +2827,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2314,13 +2846,13 @@
         <v>41</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>141</v>
       </c>
@@ -2328,20 +2860,20 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -2352,7 +2884,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -2360,7 +2892,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -2368,7 +2900,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -2376,7 +2908,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -2384,7 +2916,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -2392,153 +2924,374 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>145</v>
+        <v>241</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>161</v>
+      <c r="A33" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>165</v>
-      </c>
-      <c r="C37" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>184</v>
-      </c>
-      <c r="C39" t="s">
-        <v>186</v>
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>182</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C40" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C42" t="s">
+      <c r="B47" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+    <row r="50" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C50" s="10"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="C47" s="10"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>194</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C52" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>196</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C53" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>198</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="C55" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
+      <c r="C56" s="4" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>197</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="D56" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>235</v>
+      </c>
+      <c r="C60" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D62" s="12"/>
+      <c r="E62" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="J62" s="12"/>
+    </row>
+    <row r="63" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="H63" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="I63" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="J63" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C64" t="s">
+        <v>240</v>
+      </c>
+      <c r="E64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="H65" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="I65" s="16"/>
+      <c r="J65" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="66" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D66" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="67" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="G67" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="E66:I66"/>
+    <mergeCell ref="H65:I65"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D32C48-A49B-554E-9343-B59A3EBF16A1}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="32" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>201</v>
-      </c>
-      <c r="C53" t="s">
-        <v>202</v>
-      </c>
-      <c r="D53" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D59" s="2"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>216</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C416EEE-9E77-7F4A-BC4B-9ED2253E0B32}">
   <dimension ref="A1:A24"/>
   <sheetViews>
@@ -2550,87 +3303,87 @@
   <sheetData>
     <row r="1" spans="1:1" ht="32" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2638,7 +3391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9C14A1-9CE0-134D-A749-A98061352FDA}">
   <dimension ref="A1:A25"/>
   <sheetViews>
@@ -2650,67 +3403,67 @@
   <sheetData>
     <row r="1" spans="1:1" ht="32" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="24" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2718,7 +3471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA6D231-497E-7644-A54F-8490DA236801}">
   <dimension ref="A1:A75"/>
   <sheetViews>
@@ -3038,7 +3791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934508D2-8E30-6E4E-850C-7E52FEB11486}">
   <dimension ref="A1:A39"/>
   <sheetViews>

</xml_diff>